<commit_message>
add tpe.suggest parameters to config file
</commit_message>
<xml_diff>
--- a/optimization/k8s-automation/acmeair-perf.xlsx
+++ b/optimization/k8s-automation/acmeair-perf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adalbertoibm.com/Coding/Dockerized_AcmeAir/smart-tuning/optimization/k8s-automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66C954F-4E4D-9B4B-9220-46B6991BFE73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B753A8A-31ED-B84E-A540-3BB40CD6355E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="3600" windowWidth="23880" windowHeight="14320" xr2:uid="{80E45259-0848-6248-92DF-673E6A44B89B}"/>
   </bookViews>
@@ -484,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E7720D-6ADC-904B-B5BA-781B9DAB6B97}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,56 +662,85 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>766</v>
+      </c>
+      <c r="D8">
+        <v>10040</v>
+      </c>
+      <c r="E8">
+        <v>11810</v>
+      </c>
+      <c r="F8">
+        <v>829</v>
+      </c>
+      <c r="G8">
+        <v>10140</v>
+      </c>
+      <c r="H8">
+        <v>11410</v>
+      </c>
+      <c r="I8">
+        <v>13570</v>
+      </c>
+    </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>766</v>
+        <v>814</v>
       </c>
       <c r="D9">
-        <v>10040</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>11810</v>
+        <v>20</v>
       </c>
       <c r="F9">
-        <v>829</v>
+        <v>755</v>
       </c>
       <c r="G9">
-        <v>10140</v>
+        <v>9</v>
       </c>
       <c r="H9">
-        <v>11410</v>
+        <v>6</v>
       </c>
       <c r="I9">
-        <v>13570</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>814</v>
-      </c>
-      <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <v>20</v>
-      </c>
-      <c r="F10">
-        <v>755</v>
-      </c>
-      <c r="G10">
-        <v>9</v>
-      </c>
-      <c r="H10">
-        <v>6</v>
-      </c>
-      <c r="I10">
-        <v>46</v>
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -719,128 +748,99 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12">
+      <c r="C11">
         <f>256+55</f>
         <v>311</v>
       </c>
-      <c r="D12">
+      <c r="D11">
         <f>397+55</f>
         <v>452</v>
       </c>
-      <c r="E12">
+      <c r="E11">
         <f>469+69</f>
         <v>538</v>
       </c>
-      <c r="F12">
+      <c r="F11">
         <f>305+69</f>
         <v>374</v>
       </c>
-      <c r="G12">
+      <c r="G11">
         <f>448+56</f>
         <v>504</v>
       </c>
-      <c r="H12">
+      <c r="H11">
         <f>435+57</f>
         <v>492</v>
       </c>
-      <c r="I12">
+      <c r="I11">
         <f>511+71</f>
         <v>582</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <f>C8/C11</f>
+        <v>2.463022508038585</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:I12" si="0">D8/D11</f>
+        <v>22.212389380530972</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>21.951672862453531</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2.2165775401069521</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>20.11904761904762</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>23.191056910569106</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>23.31615120274914</v>
+      </c>
+    </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13">
-        <f>C9/C12</f>
-        <v>2.463022508038585</v>
+        <f>C9/C8</f>
+        <v>1.0626631853785902</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:I13" si="0">D9/D12</f>
-        <v>22.212389380530972</v>
+        <f t="shared" ref="D13:G13" si="1">D9/D8</f>
+        <v>7.9681274900398409E-4</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>21.951672862453531</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>2.2165775401069521</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>20.11904761904762</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>23.191056910569106</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>23.31615120274914</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14">
-        <f>C10/C9</f>
-        <v>1.0626631853785902</v>
-      </c>
-      <c r="D14">
-        <f t="shared" ref="D14:G14" si="1">D10/D9</f>
-        <v>7.9681274900398409E-4</v>
-      </c>
-      <c r="E14">
         <f t="shared" si="1"/>
         <v>1.693480101608806E-3</v>
       </c>
-      <c r="F14">
+      <c r="F13">
         <f t="shared" si="1"/>
         <v>0.9107358262967431</v>
       </c>
-      <c r="G14">
+      <c r="G13">
         <f t="shared" si="1"/>
         <v>8.8757396449704138E-4</v>
       </c>
-      <c r="H14">
-        <f t="shared" ref="H14:I14" si="2">H10/H9</f>
+      <c r="H13">
+        <f t="shared" ref="H13:I13" si="2">H9/H8</f>
         <v>5.258545135845749E-4</v>
       </c>
-      <c r="I14">
+      <c r="I13">
         <f t="shared" si="2"/>
         <v>3.3898305084745762E-3</v>
       </c>

</xml_diff>